<commit_message>
streaming compaction with three execution models
</commit_message>
<xml_diff>
--- a/SC/SC_data.xlsx
+++ b/SC/SC_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="250">
   <si>
     <t>ALUTs</t>
   </si>
@@ -835,7 +835,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>b+27:45asic(not_use_pmem)</t>
+    <t>ul16_1_cu2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ul32_1_cu2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_no_pmem</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1293,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -1879,8 +1887,8 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
-        <v>13</v>
+      <c r="A20" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>183</v>
@@ -1915,8 +1923,8 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
-        <v>14</v>
+      <c r="A21" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>198</v>
@@ -1998,7 +2006,7 @@
     </row>
     <row r="27" spans="1:14" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="1">

</xml_diff>